<commit_message>
Added product class and update login
</commit_message>
<xml_diff>
--- a/FlipkartWebAutomation/src/main/java/com/flipkart/testdata/TestingData.xlsx
+++ b/FlipkartWebAutomation/src/main/java/com/flipkart/testdata/TestingData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>testData</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>Electronics</t>
+  </si>
+  <si>
+    <t>Mobiles</t>
+  </si>
+  <si>
+    <t>Men</t>
+  </si>
+  <si>
+    <t>productName</t>
   </si>
 </sst>
 </file>
@@ -387,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -456,7 +465,15 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the testCase of Applemob
</commit_message>
<xml_diff>
--- a/FlipkartWebAutomation/src/main/java/com/flipkart/testdata/TestingData.xlsx
+++ b/FlipkartWebAutomation/src/main/java/com/flipkart/testdata/TestingData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>testData</t>
   </si>
@@ -78,7 +78,23 @@
     <t>productTypeName</t>
   </si>
   <si>
-    <t>OPPO</t>
+    <t>Samsung</t>
+  </si>
+  <si>
+    <t>samsungPageVerificationMessage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samsung Mobile Phones
+</t>
+  </si>
+  <si>
+    <t>AppleMobPageVerificationMessage</t>
+  </si>
+  <si>
+    <t>Apple Store</t>
+  </si>
+  <si>
+    <t>Apple</t>
   </si>
 </sst>
 </file>
@@ -396,16 +412,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31.83203125" customWidth="1"/>
+    <col min="1" max="1" width="29.83203125" customWidth="1"/>
+    <col min="2" max="2" width="33.5" customWidth="1"/>
     <col min="3" max="3" width="21.83203125" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" customWidth="1"/>
     <col min="5" max="5" width="21.5" customWidth="1"/>
@@ -475,6 +491,25 @@
       <c r="B7" t="s">
         <v>16</v>
       </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added library of beseBattery
</commit_message>
<xml_diff>
--- a/FlipkartWebAutomation/src/main/java/com/flipkart/testdata/TestingData.xlsx
+++ b/FlipkartWebAutomation/src/main/java/com/flipkart/testdata/TestingData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>testData</t>
   </si>
@@ -95,19 +95,39 @@
   </si>
   <si>
     <t>Apple</t>
+  </si>
+  <si>
+    <t>bestBatteryPhones</t>
+  </si>
+  <si>
+    <t>Infinix Hot 9 (Violet, 64 GB)</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy M11 (Black, 32 GB)</t>
+  </si>
+  <si>
+    <t>Motorola G8 Power Lite (Royal Blue, 64 GB)</t>
+  </si>
+  <si>
+    <t>Motorola Edge+ (Thunder Grey, 256 GB)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Menlo"/>
     </font>
   </fonts>
   <fills count="2">
@@ -130,11 +150,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,19 +433,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.83203125" customWidth="1"/>
     <col min="2" max="2" width="33.5" customWidth="1"/>
-    <col min="3" max="3" width="21.83203125" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" customWidth="1"/>
-    <col min="5" max="5" width="21.5" customWidth="1"/>
+    <col min="3" max="3" width="40.1640625" customWidth="1"/>
+    <col min="4" max="4" width="51.33203125" customWidth="1"/>
+    <col min="5" max="5" width="42" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -511,6 +532,23 @@
         <v>20</v>
       </c>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>